<commit_message>
apart from arrays, all stack allocated
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Investimentos\Obrigações\Manuel\42 Lisbon\CURSUS\minishell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D867CA-8A55-446E-B588-788613A4EEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AD536E-F0A1-47ED-B722-2D74E5B28A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>test</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>echo hello &gt;"test1"</t>
+  </si>
+  <si>
+    <t>cat split_* | grep 'block-&gt;' &gt;test1 &amp;&amp; cat test1</t>
+  </si>
+  <si>
+    <t>echo "hello""bye"</t>
   </si>
 </sst>
 </file>
@@ -380,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:H11"/>
+  <dimension ref="B3:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +444,18 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>